<commit_message>
Aulas do primeiro módulo - copiar e colar (explicação)
</commit_message>
<xml_diff>
--- a/aula-copiar-colar.xlsx
+++ b/aula-copiar-colar.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\02 Primeiros passos sobre planilha eletrônica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas-Resultado Final" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>RELATÓRIO DE VENDAS</t>
   </si>
@@ -69,24 +69,19 @@
   </si>
   <si>
     <t>Venda média</t>
+  </si>
+  <si>
+    <t>Colocar os dados organizados em horizontal na vertical: Seleciona os campos desejados, clica na célula onde pretende colar os dados. Clica na aba colar/colar especial/ seleciona os tipos e formatos desejados e por fim clica em transpor e ok. O mesmo vale para a operação inversa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;#,##0.00"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +105,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -157,18 +174,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -181,25 +197,33 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,14 +536,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G28"/>
+  <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="7" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="19.5" x14ac:dyDescent="0.3">
@@ -553,10 +580,10 @@
       <c r="C4" s="6">
         <v>183</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>3375</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <f>D4/C4</f>
         <v>18.442622950819672</v>
       </c>
@@ -568,10 +595,10 @@
       <c r="C5" s="8">
         <v>116</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="14">
         <v>9293</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <f t="shared" ref="E5:E8" si="0">D5/C5</f>
         <v>80.112068965517238</v>
       </c>
@@ -583,10 +610,10 @@
       <c r="C6" s="8">
         <v>179</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>3936</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <f t="shared" si="0"/>
         <v>21.988826815642458</v>
       </c>
@@ -598,10 +625,10 @@
       <c r="C7" s="8">
         <v>81</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>6034</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <f t="shared" si="0"/>
         <v>74.493827160493822</v>
       </c>
@@ -613,10 +640,10 @@
       <c r="C8" s="10">
         <v>77</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="15">
         <v>5159</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="15">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
@@ -646,41 +673,86 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6">
+        <v>183</v>
+      </c>
+      <c r="D15" s="23">
+        <v>3375</v>
+      </c>
+      <c r="E15" s="13">
+        <f>D15/C15</f>
+        <v>18.442622950819672</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="B16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="8">
+        <v>116</v>
+      </c>
+      <c r="D16" s="24">
+        <v>9293</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" ref="E16:E19" si="1">D16/C16</f>
+        <v>80.112068965517238</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="B17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="8">
+        <v>179</v>
+      </c>
+      <c r="D17" s="24">
+        <v>3936</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="1"/>
+        <v>21.988826815642458</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="8">
+        <v>81</v>
+      </c>
+      <c r="D18" s="14">
+        <v>6034</v>
+      </c>
+      <c r="E18" s="14">
+        <f t="shared" si="1"/>
+        <v>74.493827160493822</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="B19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="10">
+        <v>77</v>
+      </c>
+      <c r="D19" s="25">
+        <v>5159</v>
+      </c>
+      <c r="E19" s="15">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
     </row>
     <row r="24" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4">
@@ -689,44 +761,100 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
+      <c r="C25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="17">
+        <v>183</v>
+      </c>
+      <c r="D26" s="17">
+        <v>116</v>
+      </c>
+      <c r="E26" s="17">
+        <v>179</v>
+      </c>
+      <c r="F26" s="17">
+        <v>81</v>
+      </c>
+      <c r="G26" s="17">
+        <v>77</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+      <c r="C27" s="20">
+        <v>3375</v>
+      </c>
+      <c r="D27" s="20">
+        <v>9293</v>
+      </c>
+      <c r="E27" s="20">
+        <v>3936</v>
+      </c>
+      <c r="F27" s="20">
+        <v>6034</v>
+      </c>
+      <c r="G27" s="20">
+        <v>5159</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="C28" s="21">
+        <f>C27/C26</f>
+        <v>18.442622950819672</v>
+      </c>
+      <c r="D28" s="21">
+        <f>D27/D26</f>
+        <v>80.112068965517238</v>
+      </c>
+      <c r="E28" s="21">
+        <f>E27/E26</f>
+        <v>21.988826815642458</v>
+      </c>
+      <c r="F28" s="21">
+        <f>F27/F26</f>
+        <v>74.493827160493822</v>
+      </c>
+      <c r="G28" s="21">
+        <f>G27/G26</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B31:E31"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>